<commit_message>
DOMA-2542 Localization for Excel template (ticket_report_status_executor)
</commit_message>
<xml_diff>
--- a/apps/condo/domains/ticket/templates/TicketAnalyticsExportTemplate[property_status].xlsx
+++ b/apps/condo/domains/ticket/templates/TicketAnalyticsExportTemplate[property_status].xlsx
@@ -55,25 +55,25 @@
     <t>{d.tickets[i].new_or_reopened}</t>
   </si>
   <si>
-    <t>{d.tickets[i + 1].address}</t>
-  </si>
-  <si>
-    <t>{d.tickets[i + 1].processing}</t>
-  </si>
-  <si>
-    <t>{d.tickets[i + 1].completed}</t>
-  </si>
-  <si>
-    <t>{d.tickets[i + 1].canceled}</t>
-  </si>
-  <si>
-    <t>{d.tickets[i + 1].deferred}</t>
-  </si>
-  <si>
-    <t>{d.tickets[i + 1].closed}</t>
-  </si>
-  <si>
-    <t>{d.tickets[i + 1].new_or_reopened}</t>
+    <t>{d.tickets[i+1].address}</t>
+  </si>
+  <si>
+    <t>{d.tickets[i+1].processing}</t>
+  </si>
+  <si>
+    <t>{d.tickets[i+1].completed}</t>
+  </si>
+  <si>
+    <t>{d.tickets[i+1].canceled}</t>
+  </si>
+  <si>
+    <t>{d.tickets[i+1].deferred}</t>
+  </si>
+  <si>
+    <t>{d.tickets[i+1].closed}</t>
+  </si>
+  <si>
+    <t>{d.tickets[i+1].new_or_reopened}</t>
   </si>
 </sst>
 </file>
@@ -385,13 +385,7 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -490,10 +484,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -748,13 +742,7 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
+        <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -1067,10 +1055,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">

</xml_diff>

<commit_message>
Revert "DOMA-2542 Localization for Excel template (ticket_report_status_executor)"
This reverts commit af4ec5a693738089a0e025afe5e6f4afde0035e8.
</commit_message>
<xml_diff>
--- a/apps/condo/domains/ticket/templates/TicketAnalyticsExportTemplate[property_status].xlsx
+++ b/apps/condo/domains/ticket/templates/TicketAnalyticsExportTemplate[property_status].xlsx
@@ -55,25 +55,25 @@
     <t>{d.tickets[i].new_or_reopened}</t>
   </si>
   <si>
-    <t>{d.tickets[i+1].address}</t>
-  </si>
-  <si>
-    <t>{d.tickets[i+1].processing}</t>
-  </si>
-  <si>
-    <t>{d.tickets[i+1].completed}</t>
-  </si>
-  <si>
-    <t>{d.tickets[i+1].canceled}</t>
-  </si>
-  <si>
-    <t>{d.tickets[i+1].deferred}</t>
-  </si>
-  <si>
-    <t>{d.tickets[i+1].closed}</t>
-  </si>
-  <si>
-    <t>{d.tickets[i+1].new_or_reopened}</t>
+    <t>{d.tickets[i + 1].address}</t>
+  </si>
+  <si>
+    <t>{d.tickets[i + 1].processing}</t>
+  </si>
+  <si>
+    <t>{d.tickets[i + 1].completed}</t>
+  </si>
+  <si>
+    <t>{d.tickets[i + 1].canceled}</t>
+  </si>
+  <si>
+    <t>{d.tickets[i + 1].deferred}</t>
+  </si>
+  <si>
+    <t>{d.tickets[i + 1].closed}</t>
+  </si>
+  <si>
+    <t>{d.tickets[i + 1].new_or_reopened}</t>
   </si>
 </sst>
 </file>
@@ -385,7 +385,13 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -484,10 +490,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-            <a:sym typeface="Helvetica Neue"/>
+            <a:latin typeface="Cambria"/>
+            <a:ea typeface="Cambria"/>
+            <a:cs typeface="Cambria"/>
+            <a:sym typeface="Cambria"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -742,7 +748,13 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst/>
+        <a:effectLst>
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -1055,10 +1067,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-            <a:sym typeface="Helvetica Neue"/>
+            <a:latin typeface="Cambria"/>
+            <a:ea typeface="Cambria"/>
+            <a:cs typeface="Cambria"/>
+            <a:sym typeface="Cambria"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">

</xml_diff>

<commit_message>
DOMA-3100 add formatter convert to number for some colomns
</commit_message>
<xml_diff>
--- a/apps/condo/domains/ticket/templates/TicketAnalyticsExportTemplate[property_status].xlsx
+++ b/apps/condo/domains/ticket/templates/TicketAnalyticsExportTemplate[property_status].xlsx
@@ -1,17 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25423"/>
+  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{575920EE-58CA-42F4-B763-2B3C610DBBBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="191028" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>{d.i18n.address}</t>
   </si>
@@ -37,65 +53,52 @@
     <t>{d.tickets[i].address}</t>
   </si>
   <si>
-    <t>{d.tickets[i].processing}</t>
-  </si>
-  <si>
-    <t>{d.tickets[i].completed}</t>
-  </si>
-  <si>
-    <t>{d.tickets[i].canceled}</t>
-  </si>
-  <si>
-    <t>{d.tickets[i].deferred}</t>
-  </si>
-  <si>
-    <t>{d.tickets[i].closed}</t>
-  </si>
-  <si>
-    <t>{d.tickets[i].new_or_reopened}</t>
+    <t>{d.tickets[i].processing:formatN()}</t>
+  </si>
+  <si>
+    <t>{d.tickets[i].completed:formatN()}</t>
+  </si>
+  <si>
+    <t>{d.tickets[i].canceled:formatN()}</t>
+  </si>
+  <si>
+    <t>{d.tickets[i].deferred:formatN()}</t>
+  </si>
+  <si>
+    <t>{d.tickets[i].closed:formatN()}</t>
+  </si>
+  <si>
+    <t>{d.tickets[i].new_or_reopened:formatN()}</t>
   </si>
   <si>
     <t>{d.tickets[i+1].address}</t>
   </si>
   <si>
-    <t>{d.tickets[i+1].processing}</t>
-  </si>
-  <si>
-    <t>{d.tickets[i+1].completed}</t>
-  </si>
-  <si>
-    <t>{d.tickets[i+1].canceled}</t>
-  </si>
-  <si>
-    <t>{d.tickets[i+1].deferred}</t>
-  </si>
-  <si>
-    <t>{d.tickets[i+1].closed}</t>
-  </si>
-  <si>
-    <t>{d.tickets[i+1].new_or_reopened}</t>
+    <t>{d.tickets[i+1].processing:formatN()}</t>
+  </si>
+  <si>
+    <t>{d.tickets[i+1].completed:formatN()}</t>
+  </si>
+  <si>
+    <t>{d.tickets[i+1].canceled:formatN()}</t>
+  </si>
+  <si>
+    <t>{d.tickets[i+1].deferred:formatN()}</t>
+  </si>
+  <si>
+    <t>{d.tickets[i+1].closed:formatN()}</t>
+  </si>
+  <si>
+    <t>{d.tickets[i+1].new_or_reopened:formatN()}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3">
     <font>
       <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="15"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
@@ -199,62 +202,122 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+  <cellXfs count="10">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ff666666"/>
-      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FF666666"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -456,7 +519,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -475,7 +538,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -505,7 +568,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -531,7 +594,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -557,7 +620,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -583,7 +646,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -609,7 +672,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -635,7 +698,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -661,7 +724,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -687,7 +750,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -713,7 +776,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -726,9 +789,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -745,7 +814,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -764,7 +833,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -790,7 +859,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -816,7 +885,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -842,7 +911,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -868,7 +937,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -894,7 +963,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -920,7 +989,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -946,7 +1015,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -972,7 +1041,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -998,7 +1067,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1011,9 +1080,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1027,7 +1102,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1046,7 +1121,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1076,7 +1151,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1102,7 +1177,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1128,7 +1203,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1154,7 +1229,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1180,7 +1255,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1206,7 +1281,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1232,7 +1307,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1258,7 +1333,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1284,7 +1359,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1297,105 +1372,115 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:G3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="12.8" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="12.6719" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6719" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.3516" style="1" customWidth="1"/>
+    <col min="1" max="2" width="12.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.375" style="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.8516" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.1719" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="39" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:7" ht="39" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="3">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="4">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="3">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="4">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="4">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="5">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" ht="39" customHeight="1">
-      <c r="A2" t="s" s="6">
+    <row r="2" spans="1:7" ht="39" customHeight="1">
+      <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s" s="6">
+      <c r="B2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s" s="6">
+      <c r="C2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s" s="6">
+      <c r="D2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s" s="6">
+      <c r="E2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s" s="6">
+      <c r="F2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s" s="6">
+      <c r="G2" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" ht="39" customHeight="1">
-      <c r="A3" t="s" s="7">
+    <row r="3" spans="1:7" ht="39" customHeight="1">
+      <c r="A3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s" s="7">
+      <c r="B3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s" s="7">
+      <c r="C3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s" s="7">
+      <c r="D3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s" s="7">
+      <c r="E3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F3" t="s" s="7">
+      <c r="F3" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="G3" t="s" s="7">
+      <c r="G3" s="9" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511806" footer="0.511806"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="0.74791700000000005" right="0.74791700000000005" top="0.98402800000000001" bottom="0.98402800000000001" header="0.51180599999999998" footer="0.51180599999999998"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>